<commit_message>
Remove support for "(0) of" syntax for settuping up lists
This is replaced by the "list of" syntax, and means that
indexInParent and isChild can be removed.
</commit_message>
<xml_diff>
--- a/Test/TestExcelFiles/Leading Trailing Spaces .xlsx
+++ b/Test/TestExcelFiles/Leading Trailing Spaces .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A72B015B-CA50-442C-AC2F-C6A2F720E7FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{50C4C2E2-32A5-46A4-819A-FE6AC62A9764}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Specification</t>
   </si>
@@ -75,10 +75,16 @@
     <t xml:space="preserve"> TableClass- -TableClass </t>
   </si>
   <si>
-    <t xml:space="preserve"> ListProperty- -ListProperty(0)  of</t>
-  </si>
-  <si>
     <t>The dashes are so that it is easier to test for leading, trailing and enclosed spaces separately</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ListProperty- -ListProperty list  of</t>
+  </si>
+  <si>
+    <t>With Item</t>
+  </si>
+  <si>
+    <t>AnyProperty of</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1389079D-C9FD-4AFA-AFB3-2F9AFFAD165C}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +562,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -575,12 +581,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -588,7 +594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
@@ -596,50 +602,63 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>